<commit_message>
add framework and moters
</commit_message>
<xml_diff>
--- a/GPIOsetting.xlsx
+++ b/GPIOsetting.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="STM32F103" sheetId="1" r:id="rId1"/>
+    <sheet name="STM32F103C8T6" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="128">
   <si>
     <t>引脚编号</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -590,11 +590,50 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>DAC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>ADC12_IN4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIM2_CH2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIM2_CH3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIM3_CH3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIM3_CH4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPI1_SCK</t>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPI1_MISO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPI1_MOSI</t>
+  </si>
+  <si>
+    <t>SPI的OLED
+无线</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NRF_CS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NRF_CE</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -726,18 +765,9 @@
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -755,12 +785,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -772,6 +796,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1055,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1071,652 +1110,680 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="2" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
+      <c r="A3" s="3">
         <v>10</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="7" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6" t="s">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>17</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>29</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>30</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
-        <v>11</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>12</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="F12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>31</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>32</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>33</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>34</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>37</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>38</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" s="8">
+        <v>3</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="8">
         <v>19</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="B20" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>13</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="F20" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="8">
         <v>20</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="B21" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="8">
+        <v>39</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="1:7" ht="57" x14ac:dyDescent="0.2">
+      <c r="A23" s="8">
+        <v>134</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="8">
+        <v>135</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="8">
+        <v>136</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="8">
+        <v>137</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="8">
+        <v>139</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="8">
+        <v>140</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="8">
+        <v>69</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>14</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>15</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
+      <c r="F29" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A30" s="8">
+        <v>70</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>17</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>29</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>30</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>31</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
-        <v>32</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
-        <v>33</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
-        <v>34</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
-        <v>37</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="6" t="s">
+      <c r="F30" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="8">
+        <v>73</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
-        <v>38</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="13">
-        <v>46</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="13">
-        <v>47</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="13">
-        <v>48</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="13">
-        <v>133</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-    </row>
-    <row r="23" spans="1:7" ht="57" x14ac:dyDescent="0.2">
-      <c r="A23" s="13">
-        <v>134</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="13" t="s">
+      <c r="F31" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="8">
+        <v>74</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="13">
-        <v>135</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13" t="s">
+      <c r="F32" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="8">
+        <v>75</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="13">
-        <v>136</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="13">
-        <v>137</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="G26" s="15" t="s">
+      <c r="F33" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="8">
         <v>76</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="13">
-        <v>139</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13" t="s">
+      <c r="B34" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="13">
-        <v>140</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="13">
-        <v>69</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="13">
-        <v>70</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="13">
-        <v>73</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="13">
-        <v>74</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="G32" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="13">
-        <v>75</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="G33" s="15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="13">
-        <v>76</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F34" s="15" t="s">
+      <c r="F34" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="G34" s="15" t="s">
+      <c r="G34" s="10" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>